<commit_message>
sync with launcher + hotaStartingArmies is syncronized with hota 1.7.3
</commit_message>
<xml_diff>
--- a/JS - main module/Info For Devs/hota changelog.xlsx
+++ b/JS - main module/Info For Devs/hota changelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="9705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="10305" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -6699,8 +6699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6848,43 +6848,43 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>2071</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>2072</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>2073</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>2074</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>2075</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>2076</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>2077</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:1" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>2078</v>
       </c>
     </row>

</xml_diff>